<commit_message>
Added documentation for M-Machine language
</commit_message>
<xml_diff>
--- a/Docs/M_Machine_Spec.xlsx
+++ b/Docs/M_Machine_Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigil\Dropbox\Documents\Personal\Creations\Code\Myrmidon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigil\Dropbox\Documents\Personal\Creations\Code\Myrmidon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E037A1D-8053-4463-A819-FEBAB8F6D789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53719C1C-B3D4-4374-9971-7A55DA3A0618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{AC20E530-6957-42EA-AEBA-67EAE384F38D}"/>
+    <workbookView xWindow="25215" yWindow="7590" windowWidth="6225" windowHeight="10785" xr2:uid="{AC20E530-6957-42EA-AEBA-67EAE384F38D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="383">
   <si>
     <t>Instruction</t>
   </si>
@@ -111,12 +111,6 @@
     <t>08</t>
   </si>
   <si>
-    <t>def xx</t>
-  </si>
-  <si>
-    <t>Define routine xx (but do not run it)</t>
-  </si>
-  <si>
     <t>09</t>
   </si>
   <si>
@@ -126,12 +120,6 @@
     <t>break</t>
   </si>
   <si>
-    <t>call xx</t>
-  </si>
-  <si>
-    <t>Call routine xx and return here after</t>
-  </si>
-  <si>
     <t>0a</t>
   </si>
   <si>
@@ -825,9 +813,6 @@
     <t>70</t>
   </si>
   <si>
-    <t>Wait for the end of the current frame (1/30 s)</t>
-  </si>
-  <si>
     <t>71</t>
   </si>
   <si>
@@ -840,9 +825,6 @@
     <t>Delay xxxx milliseconds</t>
   </si>
   <si>
-    <t>print</t>
-  </si>
-  <si>
     <t>Read a page of ROM indexed by register xx and overwrite the page at pointer yy</t>
   </si>
   <si>
@@ -1174,6 +1156,30 @@
   </si>
   <si>
     <t>Convert register xx (signed) to a string and store it in 4 words at pointer yy</t>
+  </si>
+  <si>
+    <t>def NAME</t>
+  </si>
+  <si>
+    <t>call NAME</t>
+  </si>
+  <si>
+    <t>Define routine (but do not run it)</t>
+  </si>
+  <si>
+    <t>Call routine and return here after</t>
+  </si>
+  <si>
+    <t>print xx</t>
+  </si>
+  <si>
+    <t>Wait for the end of the current frame. The ms / frame is given by xx, or 33 if xx is zero</t>
+  </si>
+  <si>
+    <t>itoa xx yyyy</t>
+  </si>
+  <si>
+    <t>sitoa xx yyyy</t>
   </si>
 </sst>
 </file>
@@ -1548,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91769CA7-8760-4F99-86F3-745C9AD69B55}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F127" sqref="F127"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1621,7 +1627,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1644,7 +1650,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1667,7 +1673,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,7 +1696,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1707,10 +1713,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1727,13 +1733,13 @@
         <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1750,13 +1756,13 @@
         <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,18 +1779,18 @@
         <v>23</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>375</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>377</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -1796,15 +1802,15 @@
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>376</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>32</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -1816,18 +1822,18 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -1839,18 +1845,18 @@
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -1862,18 +1868,18 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -1885,35 +1891,35 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
@@ -1925,18 +1931,18 @@
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>269</v>
+        <v>379</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1950,12 +1956,12 @@
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>11</v>
@@ -1964,18 +1970,18 @@
         <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>11</v>
@@ -1984,21 +1990,21 @@
         <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>11</v>
@@ -2007,21 +2013,21 @@
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>11</v>
@@ -2030,21 +2036,21 @@
         <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>11</v>
@@ -2053,18 +2059,18 @@
         <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>11</v>
@@ -2073,18 +2079,18 @@
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>11</v>
@@ -2093,18 +2099,18 @@
         <v>23</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
@@ -2113,21 +2119,21 @@
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>11</v>
@@ -2136,21 +2142,21 @@
         <v>23</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>11</v>
@@ -2159,21 +2165,21 @@
         <v>23</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>11</v>
@@ -2182,18 +2188,18 @@
         <v>23</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>11</v>
@@ -2202,21 +2208,21 @@
         <v>23</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>11</v>
@@ -2225,18 +2231,18 @@
         <v>23</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>11</v>
@@ -2245,21 +2251,21 @@
         <v>23</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>11</v>
@@ -2268,18 +2274,18 @@
         <v>23</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
@@ -2288,18 +2294,18 @@
         <v>23</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>11</v>
@@ -2308,18 +2314,18 @@
         <v>23</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>11</v>
@@ -2328,21 +2334,21 @@
         <v>23</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>11</v>
@@ -2351,21 +2357,21 @@
         <v>23</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
@@ -2374,21 +2380,21 @@
         <v>23</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>11</v>
@@ -2397,21 +2403,21 @@
         <v>23</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>11</v>
@@ -2420,21 +2426,21 @@
         <v>23</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>11</v>
@@ -2443,18 +2449,18 @@
         <v>23</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>11</v>
@@ -2463,21 +2469,21 @@
         <v>23</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>11</v>
@@ -2486,21 +2492,21 @@
         <v>23</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>11</v>
@@ -2509,21 +2515,21 @@
         <v>23</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>11</v>
@@ -2532,21 +2538,21 @@
         <v>23</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>11</v>
@@ -2555,21 +2561,21 @@
         <v>23</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>11</v>
@@ -2578,21 +2584,21 @@
         <v>23</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>11</v>
@@ -2601,21 +2607,21 @@
         <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>11</v>
@@ -2624,18 +2630,18 @@
         <v>23</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>11</v>
@@ -2647,18 +2653,18 @@
         <v>4</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,12 +2678,12 @@
         <v>2</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>11</v>
@@ -2689,15 +2695,15 @@
         <v>4</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>11</v>
@@ -2709,10 +2715,10 @@
         <v>23</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2729,15 +2735,15 @@
         <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>11</v>
@@ -2749,15 +2755,15 @@
         <v>23</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>11</v>
@@ -2769,13 +2775,13 @@
         <v>4</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2792,18 +2798,18 @@
         <v>23</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
@@ -2815,15 +2821,15 @@
         <v>4</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -2835,15 +2841,15 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>4</v>
@@ -2855,15 +2861,15 @@
         <v>4</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>4</v>
@@ -2875,15 +2881,15 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -2895,18 +2901,18 @@
         <v>4</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -2918,18 +2924,18 @@
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>11</v>
@@ -2941,18 +2947,18 @@
         <v>4</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>11</v>
@@ -2964,18 +2970,18 @@
         <v>23</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>11</v>
@@ -2987,18 +2993,18 @@
         <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>11</v>
@@ -3010,18 +3016,18 @@
         <v>23</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>11</v>
@@ -3033,15 +3039,15 @@
         <v>4</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>11</v>
@@ -3053,18 +3059,18 @@
         <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>11</v>
@@ -3076,15 +3082,15 @@
         <v>4</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>11</v>
@@ -3096,15 +3102,15 @@
         <v>4</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3118,55 +3124,55 @@
         <v>2</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E81" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>11</v>
@@ -3178,18 +3184,18 @@
         <v>4</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>11</v>
@@ -3201,15 +3207,15 @@
         <v>4</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>11</v>
@@ -3221,15 +3227,15 @@
         <v>4</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>11</v>
@@ -3241,15 +3247,15 @@
         <v>4</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>11</v>
@@ -3258,21 +3264,21 @@
         <v>23</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>11</v>
@@ -3284,18 +3290,18 @@
         <v>4</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>11</v>
@@ -3307,18 +3313,18 @@
         <v>4</v>
       </c>
       <c r="E89" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>11</v>
@@ -3330,15 +3336,15 @@
         <v>4</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>11</v>
@@ -3350,15 +3356,15 @@
         <v>4</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>11</v>
@@ -3367,21 +3373,21 @@
         <v>23</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>11</v>
@@ -3393,15 +3399,15 @@
         <v>4</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>11</v>
@@ -3410,21 +3416,21 @@
         <v>23</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>11</v>
@@ -3433,21 +3439,21 @@
         <v>23</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>4</v>
@@ -3459,15 +3465,15 @@
         <v>23</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>11</v>
@@ -3476,21 +3482,21 @@
         <v>23</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>11</v>
@@ -3499,21 +3505,21 @@
         <v>23</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E99" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="G99" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>4</v>
@@ -3525,15 +3531,15 @@
         <v>4</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>4</v>
@@ -3545,15 +3551,15 @@
         <v>11</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3569,10 +3575,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>4</v>
@@ -3581,15 +3587,15 @@
         <v>4</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>264</v>
+        <v>380</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>4</v>
@@ -3601,15 +3607,15 @@
         <v>4</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>4</v>
@@ -3621,15 +3627,15 @@
         <v>11</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3645,7 +3651,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>11</v>
@@ -3657,15 +3663,15 @@
         <v>4</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>11</v>
@@ -3677,15 +3683,15 @@
         <v>23</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>11</v>
@@ -3697,15 +3703,15 @@
         <v>4</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>11</v>
@@ -3717,15 +3723,15 @@
         <v>23</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>11</v>
@@ -3737,15 +3743,15 @@
         <v>4</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>11</v>
@@ -3757,15 +3763,15 @@
         <v>23</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3781,7 +3787,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>4</v>
@@ -3793,15 +3799,15 @@
         <v>4</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>4</v>
@@ -3813,15 +3819,15 @@
         <v>11</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>11</v>
@@ -3833,15 +3839,15 @@
         <v>4</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>11</v>
@@ -3853,15 +3859,15 @@
         <v>4</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>11</v>
@@ -3873,15 +3879,15 @@
         <v>4</v>
       </c>
       <c r="E124" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>11</v>
@@ -3893,15 +3899,15 @@
         <v>4</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>11</v>
@@ -3910,18 +3916,18 @@
         <v>23</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -3937,7 +3943,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>11</v>
@@ -3949,18 +3955,18 @@
         <v>4</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>11</v>
@@ -3972,15 +3978,15 @@
         <v>23</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>11</v>
@@ -3992,15 +3998,15 @@
         <v>4</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>11</v>
@@ -4012,15 +4018,15 @@
         <v>23</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>11</v>
@@ -4032,15 +4038,15 @@
         <v>4</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>11</v>
@@ -4052,15 +4058,15 @@
         <v>4</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4076,7 +4082,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>11</v>
@@ -4088,15 +4094,15 @@
         <v>4</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>11</v>
@@ -4108,10 +4114,10 @@
         <v>23</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial commit of v1.1 sound update, documentation to follow
</commit_message>
<xml_diff>
--- a/Docs/M_Machine_Spec.xlsx
+++ b/Docs/M_Machine_Spec.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigil\Dropbox\Documents\Personal\Creations\Code\Myrmidon\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Documents\Personal\Creations\Code\Myrmidon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53719C1C-B3D4-4374-9971-7A55DA3A0618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D0B35-9687-4F51-ADFE-5344617DBAF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25215" yWindow="7590" windowWidth="6225" windowHeight="10785" xr2:uid="{AC20E530-6957-42EA-AEBA-67EAE384F38D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC20E530-6957-42EA-AEBA-67EAE384F38D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="399">
   <si>
     <t>Instruction</t>
   </si>
@@ -1180,6 +1180,54 @@
   </si>
   <si>
     <t>sitoa xx yyyy</t>
+  </si>
+  <si>
+    <t>SOUND AND MUSIC</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>playsnd xx yyyy</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>stopsnd xx</t>
+  </si>
+  <si>
+    <t>loadsnd xxxx</t>
+  </si>
+  <si>
+    <t>Load sound stored in the page at address xxxx, setting up the pattern list</t>
+  </si>
+  <si>
+    <t>loadsnd xx</t>
+  </si>
+  <si>
+    <t>Load sound stored in the page at pointer xxxx, setting up the pattern list</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>playsnd xx yy</t>
+  </si>
+  <si>
+    <t>Play the pattern indexed by register yy using the playhead given by register xx (0 or 1)</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>Play pattern yyyy using the playhead given by register xx (0 or 1)</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>Stop the playhead given by register xx (0 or 1)</t>
   </si>
 </sst>
 </file>
@@ -1552,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91769CA7-8760-4F99-86F3-745C9AD69B55}">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,7 +4114,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>324</v>
+        <v>383</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4082,41 +4130,157 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>325</v>
+        <v>384</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>326</v>
+        <v>390</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>328</v>
+        <v>391</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E140" s="1" t="s">
+      <c r="B148" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E148" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F140" s="1" t="s">
+      <c r="F148" s="1" t="s">
         <v>329</v>
       </c>
     </row>

</xml_diff>